<commit_message>
Add support to validation tool to dynmically push patient data into the spreedsheet to compute patient specific validation values Add support to run validation on a given directory with expected files, along with the V&V test generated fileset
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/PatientValidationData.xlsx
+++ b/data/human/adult/validation/PatientValidationData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Programming\Pulse\engine-ingmar\test\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\engine\data\human\adult\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3A68A3-9A58-495B-B620-A3499CA9C4F1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A687EA-5535-45F4-97B9-878D05B8FDCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="724" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="32620" windowHeight="21100" tabRatio="724" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patient-Validation" sheetId="33" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="68">
   <si>
     <t>Output</t>
   </si>
@@ -218,6 +218,12 @@
   </si>
   <si>
     <t>kg</t>
+  </si>
+  <si>
+    <t>Male Multiplier</t>
+  </si>
+  <si>
+    <t>Female Multiplier</t>
   </si>
 </sst>
 </file>
@@ -1238,31 +1244,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L14" sqref="L14"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="39" style="4" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="4.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="4"/>
+    <col min="2" max="2" width="7.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="14" style="13" customWidth="1"/>
+    <col min="6" max="6" width="20.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.7265625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="4.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" style="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.54296875" style="21" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1272,211 +1280,239 @@
       <c r="C1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="26"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="26"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="26"/>
-    </row>
-    <row r="4" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="26"/>
+    </row>
+    <row r="4" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="26"/>
-    </row>
-    <row r="5" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="26"/>
+    </row>
+    <row r="5" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="26"/>
-    </row>
-    <row r="6" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="26"/>
+    </row>
+    <row r="6" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="26"/>
-    </row>
-    <row r="7" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="26"/>
+    </row>
+    <row r="7" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="19"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="G7" s="19"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="26"/>
-    </row>
-    <row r="8" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="26"/>
+    </row>
+    <row r="8" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>45</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="20"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="26"/>
-    </row>
-    <row r="9" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="26"/>
+    </row>
+    <row r="9" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="26"/>
-    </row>
-    <row r="10" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="26"/>
+    </row>
+    <row r="10" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="26"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="26"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>48</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="20"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="18"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="18"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="26"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="26"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="18"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="G12" s="18"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="26"/>
-    </row>
-    <row r="13" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="26"/>
+    </row>
+    <row r="13" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>64</v>
       </c>
@@ -1486,71 +1522,79 @@
       <c r="C13" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="26" t="s">
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="19"/>
-      <c r="D14" s="3"/>
+      <c r="D14" s="19"/>
       <c r="E14" s="19"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="23"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="26"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="26"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="26"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="26"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="26"/>
-    </row>
-    <row r="17" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="26"/>
+    </row>
+    <row r="17" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
         <v>27</v>
       </c>
@@ -1560,23 +1604,25 @@
       <c r="C17" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="26" t="s">
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
         <v>56</v>
       </c>
@@ -1586,23 +1632,25 @@
       <c r="C18" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="H18" s="18"/>
       <c r="I18" s="3"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="26" t="s">
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
         <v>28</v>
       </c>
@@ -1612,23 +1660,25 @@
       <c r="C19" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="26" t="s">
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>17</v>
       </c>
@@ -1638,23 +1688,25 @@
       <c r="C20" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="G20" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="26" t="s">
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="26" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>20</v>
       </c>
@@ -1664,23 +1716,25 @@
       <c r="C21" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="G21" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="26" t="s">
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
         <v>36</v>
       </c>
@@ -1690,23 +1744,25 @@
       <c r="C22" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="G22" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="26" t="s">
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="26" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
         <v>22</v>
       </c>
@@ -1716,23 +1772,25 @@
       <c r="C23" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="G23" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="26" t="s">
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
         <v>23</v>
       </c>
@@ -1742,23 +1800,25 @@
       <c r="C24" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="G24" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F24" s="15"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
+      <c r="H24" s="15"/>
       <c r="I24" s="3"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="26" t="s">
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="26" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="8" customFormat="1" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="8" customFormat="1" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
         <v>29</v>
       </c>
@@ -1768,25 +1828,27 @@
       <c r="C25" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="G25" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F25" s="23"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="23"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="I25" s="3"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="26" t="s">
+      <c r="K25" s="3"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="26" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
         <v>30</v>
       </c>
@@ -1796,23 +1858,25 @@
       <c r="C26" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="G26" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F26" s="18"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="22"/>
+      <c r="H26" s="18"/>
       <c r="I26" s="3"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="26" t="s">
+      <c r="J26" s="22"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="26" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
         <v>18</v>
       </c>
@@ -1822,25 +1886,27 @@
       <c r="C27" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="G27" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="23"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3" t="s">
+      <c r="H27" s="23"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="I27" s="3"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="26" t="s">
+      <c r="K27" s="3"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="26" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
         <v>19</v>
       </c>
@@ -1850,25 +1916,27 @@
       <c r="C28" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F28" s="23"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3" t="s">
+      <c r="H28" s="23"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="I28" s="3"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="26" t="s">
+      <c r="K28" s="3"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="26" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
         <v>21</v>
       </c>
@@ -1878,25 +1946,27 @@
       <c r="C29" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="G29" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F29" s="23"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="11" t="s">
+      <c r="H29" s="23"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="I29" s="3"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="26" t="s">
+      <c r="K29" s="3"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="26" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
         <v>24</v>
       </c>
@@ -1906,25 +1976,27 @@
       <c r="C30" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="23"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="11" t="s">
+      <c r="H30" s="23"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="I30" s="3"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="26" t="s">
+      <c r="K30" s="3"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="26" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
         <v>25</v>
       </c>
@@ -1934,19 +2006,21 @@
       <c r="C31" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D31" s="20" t="s">
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="G31" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F31" s="18"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="22"/>
+      <c r="H31" s="18"/>
       <c r="I31" s="3"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="26" t="s">
+      <c r="J31" s="22"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="26" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update logic for patient generation for our variability study
Add a few setup patient properties to the patient
Tracking error milestones (if we hit them)
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/PatientValidationData.xlsx
+++ b/data/human/adult/validation/PatientValidationData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\engine\data\human\adult\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A687EA-5535-45F4-97B9-878D05B8FDCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF000F4-6778-4583-B338-9EB8E419CB40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="32620" windowHeight="21100" tabRatio="724" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11040" yWindow="2930" windowWidth="14670" windowHeight="10580" tabRatio="724" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patient-Validation" sheetId="33" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="68">
   <si>
     <t>Output</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Height*</t>
   </si>
   <si>
-    <t>CarinaToTeethDistance*</t>
-  </si>
-  <si>
     <t>HeartRateBaseline</t>
   </si>
   <si>
@@ -214,16 +211,19 @@
     <t>3f</t>
   </si>
   <si>
-    <t>IdealBodyWeight</t>
-  </si>
-  <si>
-    <t>kg</t>
-  </si>
-  <si>
     <t>Male Multiplier</t>
   </si>
   <si>
     <t>Female Multiplier</t>
+  </si>
+  <si>
+    <t>PulsePressureBaseline*</t>
+  </si>
+  <si>
+    <t>BodyMassIndex*</t>
+  </si>
+  <si>
+    <t>IdealBodyWeight*</t>
   </si>
 </sst>
 </file>
@@ -1244,11 +1244,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="topRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1278,13 +1278,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>2</v>
@@ -1305,13 +1305,13 @@
         <v>5</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
@@ -1334,7 +1334,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -1406,7 +1406,7 @@
     </row>
     <row r="7" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -1424,7 +1424,7 @@
     </row>
     <row r="8" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="20"/>
@@ -1442,7 +1442,7 @@
     </row>
     <row r="9" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -1460,10 +1460,10 @@
     </row>
     <row r="10" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
+        <v>66</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="3"/>
@@ -1472,13 +1472,13 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="14"/>
+      <c r="L10" s="3"/>
       <c r="M10" s="20"/>
       <c r="N10" s="26"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="20"/>
@@ -1496,7 +1496,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -1513,23 +1513,15 @@
       <c r="N12" s="26"/>
     </row>
     <row r="13" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>10</v>
-      </c>
+      <c r="A13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
-      <c r="F13" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="F13" s="20"/>
+      <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -1537,12 +1529,12 @@
       <c r="L13" s="14"/>
       <c r="M13" s="20"/>
       <c r="N13" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="19"/>
@@ -1560,7 +1552,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
@@ -1578,7 +1570,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
@@ -1596,21 +1588,21 @@
     </row>
     <row r="17" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="20"/>
       <c r="F17" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -1619,26 +1611,26 @@
       <c r="L17" s="3"/>
       <c r="M17" s="20"/>
       <c r="N17" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
       <c r="F18" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H18" s="18"/>
       <c r="I18" s="3"/>
@@ -1647,26 +1639,26 @@
       <c r="L18" s="14"/>
       <c r="M18" s="20"/>
       <c r="N18" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
       <c r="F19" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -1675,26 +1667,26 @@
       <c r="L19" s="14"/>
       <c r="M19" s="20"/>
       <c r="N19" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
       <c r="F20" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -1703,26 +1695,26 @@
       <c r="L20" s="14"/>
       <c r="M20" s="20"/>
       <c r="N20" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
       <c r="F21" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -1731,46 +1723,36 @@
       <c r="L21" s="14"/>
       <c r="M21" s="20"/>
       <c r="N21" s="26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A22" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>59</v>
-      </c>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
-      <c r="F22" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="14"/>
       <c r="M22" s="20"/>
-      <c r="N22" s="26" t="s">
-        <v>62</v>
-      </c>
+      <c r="N22" s="26"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="20"/>
@@ -1778,7 +1760,7 @@
         <v>53</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
@@ -1792,68 +1774,66 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>34</v>
+        <v>21</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
-      <c r="F24" s="17" t="s">
-        <v>57</v>
+      <c r="F24" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H24" s="15"/>
+        <v>36</v>
+      </c>
+      <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="14"/>
       <c r="M24" s="20"/>
       <c r="N24" s="26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" s="8" customFormat="1" ht="24.5" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="20" t="s">
         <v>58</v>
       </c>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="17" t="s">
+        <v>56</v>
+      </c>
       <c r="G25" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H25" s="23"/>
+        <v>36</v>
+      </c>
+      <c r="H25" s="15"/>
       <c r="I25" s="3"/>
-      <c r="J25" s="11" t="s">
-        <v>40</v>
-      </c>
+      <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="14"/>
       <c r="M25" s="20"/>
       <c r="N25" s="26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" s="8" customFormat="1" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="24" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>33</v>
       </c>
       <c r="C26" s="19" t="s">
         <v>10</v>
@@ -1861,27 +1841,29 @@
       <c r="D26" s="19"/>
       <c r="E26" s="19"/>
       <c r="F26" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H26" s="18"/>
+        <v>36</v>
+      </c>
+      <c r="H26" s="23"/>
       <c r="I26" s="3"/>
-      <c r="J26" s="22"/>
+      <c r="J26" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="K26" s="3"/>
       <c r="L26" s="14"/>
       <c r="M26" s="20"/>
       <c r="N26" s="26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>34</v>
+        <v>29</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>33</v>
       </c>
       <c r="C27" s="19" t="s">
         <v>10</v>
@@ -1889,29 +1871,27 @@
       <c r="D27" s="19"/>
       <c r="E27" s="19"/>
       <c r="F27" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H27" s="23"/>
+        <v>36</v>
+      </c>
+      <c r="H27" s="18"/>
       <c r="I27" s="3"/>
-      <c r="J27" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="J27" s="22"/>
       <c r="K27" s="3"/>
       <c r="L27" s="14"/>
       <c r="M27" s="20"/>
       <c r="N27" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" s="19" t="s">
         <v>10</v>
@@ -1919,29 +1899,29 @@
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
       <c r="F28" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H28" s="23"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K28" s="3"/>
       <c r="L28" s="14"/>
       <c r="M28" s="20"/>
       <c r="N28" s="26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="24.5" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C29" s="19" t="s">
         <v>10</v>
@@ -1949,29 +1929,29 @@
       <c r="D29" s="19"/>
       <c r="E29" s="19"/>
       <c r="F29" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H29" s="23"/>
       <c r="I29" s="3"/>
-      <c r="J29" s="11" t="s">
+      <c r="J29" s="3" t="s">
         <v>40</v>
       </c>
       <c r="K29" s="3"/>
       <c r="L29" s="14"/>
       <c r="M29" s="20"/>
       <c r="N29" s="26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" s="19" t="s">
         <v>10</v>
@@ -1979,29 +1959,29 @@
       <c r="D30" s="19"/>
       <c r="E30" s="19"/>
       <c r="F30" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H30" s="23"/>
       <c r="I30" s="3"/>
       <c r="J30" s="11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K30" s="3"/>
       <c r="L30" s="14"/>
       <c r="M30" s="20"/>
       <c r="N30" s="26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="24" t="s">
-        <v>34</v>
+        <v>23</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>33</v>
       </c>
       <c r="C31" s="19" t="s">
         <v>10</v>
@@ -2009,19 +1989,49 @@
       <c r="D31" s="19"/>
       <c r="E31" s="19"/>
       <c r="F31" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H31" s="18"/>
+        <v>36</v>
+      </c>
+      <c r="H31" s="23"/>
       <c r="I31" s="3"/>
-      <c r="J31" s="22"/>
+      <c r="J31" s="11" t="s">
+        <v>41</v>
+      </c>
       <c r="K31" s="3"/>
       <c r="L31" s="14"/>
       <c r="M31" s="20"/>
       <c r="N31" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A32" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H32" s="18"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="26" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
We need the prestabilized patient in our patient variability structure Add some notes in the Patient Validation spreedsheet to explain how validation works
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/PatientValidationData.xlsx
+++ b/data/human/adult/validation/PatientValidationData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\engine\data\human\adult\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF000F4-6778-4583-B338-9EB8E419CB40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5F457F7-A8A2-4715-9E5A-D33B31EE3D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11040" yWindow="2930" windowWidth="14670" windowHeight="10580" tabRatio="724" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="32620" windowHeight="21100" tabRatio="724" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patient-Validation" sheetId="33" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="69">
   <si>
     <t>Output</t>
   </si>
@@ -139,15 +139,6 @@
     <t>ResultsFile</t>
   </si>
   <si>
-    <t>Wikipedia - "Spirometry".  Falls just outside the limit defined by crapo1981reference</t>
-  </si>
-  <si>
-    <t>Wikipedia - "Spirometry"</t>
-  </si>
-  <si>
-    <t>Wikipedia - "Spirometry".  Falls withing limits defined by crapo1981reference</t>
-  </si>
-  <si>
     <t>MeanArterialPressure</t>
   </si>
   <si>
@@ -224,6 +215,18 @@
   </si>
   <si>
     <t>IdealBodyWeight*</t>
+  </si>
+  <si>
+    <t>PatientSpecific</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Compare the (expected) value computed by SetupPatient to the system variable in F</t>
+  </si>
+  <si>
+    <t>Compare the (expected) value computed by SetupPatient to the patient variable, which is updated every timestep in the engine</t>
   </si>
 </sst>
 </file>
@@ -791,7 +794,7 @@
     <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -850,9 +853,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1244,11 +1244,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B10" sqref="B10"/>
+      <selection pane="topRight" activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1261,16 +1261,17 @@
     <col min="6" max="6" width="20.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.81640625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7265625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="4.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" style="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.54296875" style="21" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.1796875" style="4"/>
+    <col min="9" max="9" width="12" style="2" customWidth="1"/>
+    <col min="10" max="10" width="5.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.7265625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="4.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" style="21" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.54296875" style="21" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1281,10 +1282,10 @@
         <v>32</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>2</v>
@@ -1296,25 +1297,28 @@
         <v>8</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O1" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
@@ -1329,12 +1333,13 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="26"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="M2" s="3"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="25"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -1347,10 +1352,11 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="26"/>
-    </row>
-    <row r="4" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="M3" s="3"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="25"/>
+    </row>
+    <row r="4" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>13</v>
       </c>
@@ -1365,10 +1371,11 @@
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="26"/>
-    </row>
-    <row r="5" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="M4" s="3"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="25"/>
+    </row>
+    <row r="5" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
@@ -1383,10 +1390,11 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="26"/>
-    </row>
-    <row r="6" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="M5" s="3"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="25"/>
+    </row>
+    <row r="6" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
@@ -1401,12 +1409,13 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="26"/>
-    </row>
-    <row r="7" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="M6" s="3"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="25"/>
+    </row>
+    <row r="7" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -1418,13 +1427,14 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="26"/>
-    </row>
-    <row r="8" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L7" s="3"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="25"/>
+    </row>
+    <row r="8" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="20"/>
@@ -1437,10 +1447,11 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="26"/>
-    </row>
-    <row r="9" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="M8" s="3"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="25"/>
+    </row>
+    <row r="9" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>34</v>
       </c>
@@ -1455,12 +1466,13 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="26"/>
-    </row>
-    <row r="10" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="M9" s="3"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="25"/>
+    </row>
+    <row r="10" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B10" s="20"/>
       <c r="C10" s="20"/>
@@ -1473,12 +1485,13 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="26"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="M10" s="3"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="25"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="20"/>
@@ -1490,13 +1503,14 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="26"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L11" s="3"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="25"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -1508,13 +1522,14 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="26"/>
-    </row>
-    <row r="13" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L12" s="3"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="25"/>
+    </row>
+    <row r="13" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B13" s="20"/>
       <c r="C13" s="19"/>
@@ -1526,31 +1541,33 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L13" s="3"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="25"/>
+        <v>43</v>
+      </c>
+      <c r="B14" s="24"/>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
       <c r="E14" s="19"/>
       <c r="F14" s="3"/>
       <c r="G14" s="19"/>
-      <c r="H14" s="23"/>
+      <c r="H14" s="22"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="26"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L14" s="3"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="25"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>30</v>
       </c>
@@ -1564,11 +1581,12 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="26"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L15" s="3"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="25"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>31</v>
       </c>
@@ -1582,11 +1600,12 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="26"/>
-    </row>
-    <row r="17" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L16" s="3"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="25"/>
+    </row>
+    <row r="17" spans="1:15" s="8" customFormat="1" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
         <v>26</v>
       </c>
@@ -1594,7 +1613,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="20"/>
@@ -1605,44 +1624,54 @@
         <v>36</v>
       </c>
       <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="I17" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
+      <c r="K17" s="11" t="s">
+        <v>67</v>
+      </c>
       <c r="L17" s="3"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="M17" s="3"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="20" t="s">
         <v>55</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>58</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
       <c r="F18" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H18" s="18"/>
-      <c r="I18" s="3"/>
+      <c r="I18" s="18" t="s">
+        <v>66</v>
+      </c>
       <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="K18" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="L18" s="3"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" s="8" customFormat="1" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
         <v>27</v>
       </c>
@@ -1650,27 +1679,32 @@
         <v>4</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
       <c r="F19" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="I19" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="K19" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="L19" s="3"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>16</v>
       </c>
@@ -1678,27 +1712,32 @@
         <v>11</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
       <c r="F20" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+      <c r="I20" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="K20" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="L20" s="3"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>19</v>
       </c>
@@ -1706,29 +1745,34 @@
         <v>4</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
       <c r="F21" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
+      <c r="I21" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="K21" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="L21" s="3"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
@@ -1740,11 +1784,12 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="26"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L22" s="3"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="25"/>
+    </row>
+    <row r="23" spans="1:15" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
         <v>35</v>
       </c>
@@ -1752,27 +1797,32 @@
         <v>11</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="20"/>
       <c r="F23" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+      <c r="I23" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="K23" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="L23" s="3"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="20"/>
+      <c r="O23" s="25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
         <v>21</v>
       </c>
@@ -1780,27 +1830,32 @@
         <v>4</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
       <c r="F24" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
+      <c r="I24" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="K24" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="L24" s="3"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
         <v>22</v>
       </c>
@@ -1808,27 +1863,32 @@
         <v>33</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
       <c r="F25" s="17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H25" s="15"/>
-      <c r="I25" s="3"/>
+      <c r="I25" s="18" t="s">
+        <v>66</v>
+      </c>
       <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" s="8" customFormat="1" ht="24.5" x14ac:dyDescent="0.35">
+      <c r="K25" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="L25" s="3"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="20"/>
+      <c r="O25" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" s="8" customFormat="1" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
         <v>28</v>
       </c>
@@ -1841,28 +1901,31 @@
       <c r="D26" s="19"/>
       <c r="E26" s="19"/>
       <c r="F26" s="20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H26" s="23"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="K26" s="3"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="H26" s="22"/>
+      <c r="I26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J26" s="3"/>
+      <c r="K26" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="L26" s="3"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="20"/>
+      <c r="O26" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" s="8" customFormat="1" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="23" t="s">
         <v>33</v>
       </c>
       <c r="C27" s="19" t="s">
@@ -1871,26 +1934,31 @@
       <c r="D27" s="19"/>
       <c r="E27" s="19"/>
       <c r="F27" s="20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H27" s="18"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="I27" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="J27" s="3"/>
+      <c r="K27" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="L27" s="3"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="20"/>
+      <c r="O27" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="24" t="s">
         <v>33</v>
       </c>
       <c r="C28" s="19" t="s">
@@ -1899,28 +1967,31 @@
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
       <c r="F28" s="20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H28" s="23"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K28" s="3"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="H28" s="22"/>
+      <c r="I28" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J28" s="3"/>
+      <c r="K28" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="L28" s="3"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="20"/>
+      <c r="O28" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="24" t="s">
         <v>33</v>
       </c>
       <c r="C29" s="19" t="s">
@@ -1929,28 +2000,31 @@
       <c r="D29" s="19"/>
       <c r="E29" s="19"/>
       <c r="F29" s="20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H29" s="23"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K29" s="3"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="24.5" x14ac:dyDescent="0.35">
+      <c r="H29" s="22"/>
+      <c r="I29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J29" s="3"/>
+      <c r="K29" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="L29" s="3"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="24" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="19" t="s">
@@ -1959,28 +2033,31 @@
       <c r="D30" s="19"/>
       <c r="E30" s="19"/>
       <c r="F30" s="20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H30" s="23"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="K30" s="3"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="20"/>
-      <c r="N30" s="26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H30" s="22"/>
+      <c r="I30" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J30" s="3"/>
+      <c r="K30" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="L30" s="3"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="20"/>
+      <c r="O30" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="24" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="19" t="s">
@@ -1989,28 +2066,31 @@
       <c r="D31" s="19"/>
       <c r="E31" s="19"/>
       <c r="F31" s="20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H31" s="23"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="K31" s="3"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="H31" s="22"/>
+      <c r="I31" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="K31" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="L31" s="3"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="20"/>
+      <c r="O31" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A32" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="23" t="s">
         <v>33</v>
       </c>
       <c r="C32" s="19" t="s">
@@ -2019,19 +2099,24 @@
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
       <c r="F32" s="20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H32" s="18"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="22"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="20"/>
-      <c r="N32" s="26" t="s">
-        <v>62</v>
+      <c r="I32" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="J32" s="3"/>
+      <c r="K32" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="L32" s="3"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="20"/>
+      <c r="O32" s="25" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update patient validation spreadsheet to work with other recent changes.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/PatientValidationData.xlsx
+++ b/data/human/adult/validation/PatientValidationData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\engine\data\human\adult\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\documentation\source\data\human\adult\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5F457F7-A8A2-4715-9E5A-D33B31EE3D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55D234D-1108-4AC1-9638-4E1B13F7E0ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="32620" windowHeight="21100" tabRatio="724" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29340" yWindow="3780" windowWidth="27480" windowHeight="23535" tabRatio="724" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patient-Validation" sheetId="33" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="66">
   <si>
     <t>Output</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Internal Notes</t>
   </si>
   <si>
-    <t>Mean</t>
-  </si>
-  <si>
     <t>1/min</t>
   </si>
   <si>
@@ -121,9 +118,6 @@
     <t>Algorithm</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>BodyFatFraction*</t>
   </si>
   <si>
@@ -182,9 +176,6 @@
   </si>
   <si>
     <t>TidalVolume</t>
-  </si>
-  <si>
-    <t>PatientFile</t>
   </si>
   <si>
     <t>Patient2SystemMean</t>
@@ -233,7 +224,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -391,12 +382,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -794,7 +779,7 @@
     <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -805,7 +790,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -814,10 +798,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -831,37 +811,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1246,86 +1205,85 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K31" sqref="K31"/>
+      <selection pane="topRight" activeCell="C26" sqref="C26:C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39" style="4" customWidth="1"/>
-    <col min="2" max="2" width="7.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.54296875" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.26953125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="14" style="13" customWidth="1"/>
-    <col min="6" max="6" width="20.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="14" style="10" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="2" customWidth="1"/>
-    <col min="10" max="10" width="5.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.7265625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="4.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" style="21" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.54296875" style="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.1796875" style="4"/>
+    <col min="10" max="10" width="5.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.7109375" customWidth="1"/>
+    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="C1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J1" s="5" t="s">
+      <c r="I1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
+      <c r="M1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -1334,17 +1292,17 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="25"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="15"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -1353,17 +1311,17 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="25"/>
-    </row>
-    <row r="4" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="15"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -1372,17 +1330,17 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="25"/>
-    </row>
-    <row r="5" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="15"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -1391,17 +1349,17 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="25"/>
-    </row>
-    <row r="6" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="15"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -1410,36 +1368,36 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="25"/>
-    </row>
-    <row r="7" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="15"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="19"/>
+      <c r="G7" s="12"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="25"/>
-    </row>
-    <row r="8" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="15"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1448,17 +1406,17 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="25"/>
-    </row>
-    <row r="9" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="15"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1467,17 +1425,17 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="25"/>
-    </row>
-    <row r="10" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="15"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -1486,95 +1444,95 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="25"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="15"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="18"/>
+      <c r="G11" s="11"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="25"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="15"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="18"/>
+      <c r="G12" s="11"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="25"/>
-    </row>
-    <row r="13" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="20"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="15"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="9"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="22"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="14"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="25"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="15"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1582,18 +1540,18 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="25"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A16" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="15"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -1601,183 +1559,183 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="20"/>
-      <c r="O16" s="25"/>
-    </row>
-    <row r="17" spans="1:15" s="8" customFormat="1" ht="24.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="12" t="s">
+      <c r="M16" s="3"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="15"/>
+    </row>
+    <row r="17" spans="1:15" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
+      <c r="C17" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
       <c r="F17" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J17" s="3"/>
-      <c r="K17" s="11" t="s">
-        <v>67</v>
+      <c r="K17" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
-      <c r="N17" s="20"/>
-      <c r="O17" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="24.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="10" t="s">
+      <c r="N17" s="9"/>
+      <c r="O17" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
       <c r="F18" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18" t="s">
-        <v>66</v>
+        <v>34</v>
+      </c>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="J18" s="3"/>
-      <c r="K18" s="11" t="s">
-        <v>67</v>
+      <c r="K18" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="L18" s="3"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" s="8" customFormat="1" ht="24.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="12" t="s">
+      <c r="M18" s="3"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
+      <c r="C19" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
       <c r="F19" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J19" s="3"/>
-      <c r="K19" s="11" t="s">
-        <v>67</v>
+      <c r="K19" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="L19" s="3"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="24.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
       <c r="F20" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J20" s="3"/>
-      <c r="K20" s="11" t="s">
-        <v>67</v>
+      <c r="K20" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="L20" s="3"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="24.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="12" t="s">
+      <c r="M20" s="3"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
+      <c r="C21" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
       <c r="F21" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J21" s="3"/>
-      <c r="K21" s="11" t="s">
-        <v>67</v>
+      <c r="K21" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="L21" s="3"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -1785,338 +1743,338 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="25"/>
-    </row>
-    <row r="23" spans="1:15" ht="24.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="15"/>
+    </row>
+    <row r="23" spans="1:15" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
       <c r="F23" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J23" s="3"/>
-      <c r="K23" s="11" t="s">
-        <v>67</v>
+      <c r="K23" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="L23" s="3"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="20"/>
-      <c r="O23" s="25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="24.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="12" t="s">
+      <c r="M23" s="3"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
+      <c r="C24" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
       <c r="F24" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J24" s="3"/>
-      <c r="K24" s="11" t="s">
-        <v>67</v>
+      <c r="K24" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="L24" s="3"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="20"/>
-      <c r="O24" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="36.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="10" t="s">
+      <c r="M24" s="3"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="J25" s="3"/>
+      <c r="K25" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H26" s="14"/>
+      <c r="I26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J26" s="3"/>
+      <c r="K26" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="J27" s="3"/>
+      <c r="K27" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H28" s="14"/>
+      <c r="I28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J28" s="3"/>
+      <c r="K28" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" s="14"/>
+      <c r="I29" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J29" s="3"/>
+      <c r="K29" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H30" s="14"/>
+      <c r="I30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J30" s="3"/>
+      <c r="K30" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H25" s="15"/>
-      <c r="I25" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="J25" s="3"/>
-      <c r="K25" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="L25" s="3"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="20"/>
-      <c r="O25" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" s="8" customFormat="1" ht="36.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H26" s="22"/>
-      <c r="I26" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="L26" s="3"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="20"/>
-      <c r="O26" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" s="8" customFormat="1" ht="36.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="J27" s="3"/>
-      <c r="K27" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="L27" s="3"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="20"/>
-      <c r="O27" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="36.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H28" s="22"/>
-      <c r="I28" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J28" s="3"/>
-      <c r="K28" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="L28" s="3"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="20"/>
-      <c r="O28" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="36.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H29" s="22"/>
-      <c r="I29" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J29" s="3"/>
-      <c r="K29" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="L29" s="3"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="20"/>
-      <c r="O29" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="36.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H30" s="22"/>
-      <c r="I30" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J30" s="3"/>
-      <c r="K30" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="L30" s="3"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="20"/>
-      <c r="O30" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="10" t="s">
+      <c r="B31" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H31" s="14"/>
+      <c r="I31" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="K31" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H31" s="22"/>
-      <c r="I31" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J31" s="3"/>
-      <c r="K31" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="L31" s="3"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="20"/>
-      <c r="O31" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="36.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="20" t="s">
-        <v>54</v>
+      <c r="B32" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18" t="s">
-        <v>66</v>
+        <v>34</v>
+      </c>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="J32" s="3"/>
-      <c r="K32" s="11" t="s">
-        <v>68</v>
+      <c r="K32" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="L32" s="3"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="20"/>
-      <c r="O32" s="25" t="s">
-        <v>59</v>
+      <c r="M32" s="3"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="15" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Documentation updates for next release.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/PatientValidationData.xlsx
+++ b/data/human/adult/validation/PatientValidationData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\documentation\source\data\human\adult\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55D234D-1108-4AC1-9638-4E1B13F7E0ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22088840-7D2F-4C99-A4CA-F510B1764C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29340" yWindow="3780" windowWidth="27480" windowHeight="23535" tabRatio="724" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21630" yWindow="7365" windowWidth="30555" windowHeight="21255" tabRatio="724" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patient-Validation" sheetId="33" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="65">
   <si>
     <t>Output</t>
   </si>
@@ -188,9 +188,6 @@
   </si>
   <si>
     <t>0f</t>
-  </si>
-  <si>
-    <t>3f</t>
   </si>
   <si>
     <t>Male Multiplier</t>
@@ -883,9 +880,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -923,9 +920,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -958,26 +955,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1010,26 +990,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1205,9 +1168,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C26" sqref="C26:C32"/>
+      <selection pane="topRight" activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,10 +1203,10 @@
         <v>31</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>2</v>
@@ -1255,7 +1218,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>6</v>
@@ -1430,7 +1393,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -1487,7 +1450,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="12"/>
@@ -1583,11 +1546,11 @@
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
@@ -1616,11 +1579,11 @@
       </c>
       <c r="H18" s="11"/>
       <c r="I18" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
@@ -1649,11 +1612,11 @@
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
@@ -1682,11 +1645,11 @@
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
@@ -1715,11 +1678,11 @@
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
@@ -1730,7 +1693,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -1767,11 +1730,11 @@
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
@@ -1800,11 +1763,11 @@
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
@@ -1833,17 +1796,17 @@
       </c>
       <c r="H25" s="11"/>
       <c r="I25" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J25" s="3"/>
       <c r="K25" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="9"/>
       <c r="O25" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="48.75" x14ac:dyDescent="0.25">
@@ -1866,17 +1829,17 @@
       </c>
       <c r="H26" s="14"/>
       <c r="I26" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J26" s="3"/>
       <c r="K26" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="9"/>
       <c r="O26" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="48.75" x14ac:dyDescent="0.25">
@@ -1899,17 +1862,17 @@
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J27" s="3"/>
       <c r="K27" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="9"/>
       <c r="O27" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="48.75" x14ac:dyDescent="0.25">
@@ -1932,17 +1895,17 @@
       </c>
       <c r="H28" s="14"/>
       <c r="I28" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J28" s="3"/>
       <c r="K28" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
       <c r="N28" s="9"/>
       <c r="O28" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="48.75" x14ac:dyDescent="0.25">
@@ -1965,17 +1928,17 @@
       </c>
       <c r="H29" s="14"/>
       <c r="I29" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
       <c r="N29" s="9"/>
       <c r="O29" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="48.75" x14ac:dyDescent="0.25">
@@ -1998,17 +1961,17 @@
       </c>
       <c r="H30" s="14"/>
       <c r="I30" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J30" s="3"/>
       <c r="K30" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
       <c r="N30" s="9"/>
       <c r="O30" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -2031,17 +1994,17 @@
       </c>
       <c r="H31" s="14"/>
       <c r="I31" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J31" s="3"/>
       <c r="K31" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
       <c r="N31" s="9"/>
       <c r="O31" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="48.75" x14ac:dyDescent="0.25">
@@ -2064,17 +2027,17 @@
       </c>
       <c r="H32" s="11"/>
       <c r="I32" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J32" s="3"/>
       <c r="K32" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
       <c r="N32" s="9"/>
       <c r="O32" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>